<commit_message>
code optimization, alarms added, dark colors, link checker added
</commit_message>
<xml_diff>
--- a/python/table.xlsx
+++ b/python/table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -1470,8 +1470,8 @@
   </sheetPr>
   <dimension ref="A1:DD328"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D114" activeCellId="0" sqref="D114:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>